<commit_message>
used flask.session to store session data instead of global. Should now also work with uwsgi
</commit_message>
<xml_diff>
--- a/data/web_best_plan.xlsx
+++ b/data/web_best_plan.xlsx
@@ -510,21 +510,21 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>(4,)</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>(2,)</t>
+          <t>[2]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(3, 6, 17)</t>
+          <t>[3, 6, 17]</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
         <v>2</v>
@@ -553,24 +553,24 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>(1,)</t>
+          <t>[1]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>(5, 9, 27)</t>
+          <t>[5, 9, 27]</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -596,21 +596,21 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(6,)</t>
+          <t>[6]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(2, 1, 21)</t>
+          <t>[2, 1, 21]</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
         <v>1</v>
@@ -639,21 +639,21 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>(1,)</t>
+          <t>[1]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>(5, 6, 7)</t>
+          <t>[5, 6, 7]</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
         <v>1</v>
@@ -682,24 +682,24 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>(6, 7, 23)</t>
+          <t>[6, 7, 23]</t>
         </is>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -725,24 +725,24 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>(3, 8)</t>
+          <t>[3, 8]</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>(12, 5, 25)</t>
+          <t>[12, 5, 25]</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -768,24 +768,24 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>(8,)</t>
+          <t>[8]</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>(8, 17, 23)</t>
+          <t>[8, 17, 23]</t>
         </is>
       </c>
       <c r="J8" t="n">
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -811,17 +811,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>(6,)</t>
+          <t>[6]</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>(7,)</t>
+          <t>[7]</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>(9, 27, 14)</t>
+          <t>[9, 27, 14]</t>
         </is>
       </c>
       <c r="J9" t="n">
@@ -854,24 +854,24 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>(10, 18, 19)</t>
+          <t>[10, 18, 19]</t>
         </is>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -897,17 +897,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>(11,)</t>
+          <t>[11]</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>(12, 5, 25)</t>
+          <t>[12, 5, 25]</t>
         </is>
       </c>
       <c r="J11" t="n">
@@ -940,24 +940,24 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>(10,)</t>
+          <t>[10]</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>(2, 4, 6)</t>
+          <t>[2, 4, 6]</t>
         </is>
       </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -983,24 +983,24 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>(20,)</t>
+          <t>[20]</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>(10, 18, 19)</t>
+          <t>[10, 18, 19]</t>
         </is>
       </c>
       <c r="J13" t="n">
         <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -1026,24 +1026,24 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>(5, 6, 7)</t>
+          <t>[5, 6, 7]</t>
         </is>
       </c>
       <c r="J14" t="n">
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1069,17 +1069,17 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>(1, 3, 5)</t>
+          <t>[1, 3, 5]</t>
         </is>
       </c>
       <c r="J15" t="n">
@@ -1112,24 +1112,24 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>(5, 6, 7)</t>
+          <t>[5, 6, 7]</t>
         </is>
       </c>
       <c r="J16" t="n">
         <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1155,24 +1155,24 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>(3, 6, 17)</t>
+          <t>[3, 6, 17]</t>
         </is>
       </c>
       <c r="J17" t="n">
         <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1198,24 +1198,24 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>(9, 13, 14)</t>
+          <t>[9, 13, 14]</t>
         </is>
       </c>
       <c r="J18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1241,21 +1241,21 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>(2, 1, 21)</t>
+          <t>[2, 1, 21]</t>
         </is>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
         <v>1</v>
@@ -1284,24 +1284,24 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>(7, 19, 17)</t>
+          <t>[7, 19, 17]</t>
         </is>
       </c>
       <c r="J20" t="n">
         <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -1327,24 +1327,24 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>(12,)</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>(3, 22, 1)</t>
+          <t>[3, 22, 1]</t>
         </is>
       </c>
       <c r="J21" t="n">
         <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1370,21 +1370,21 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>(3, 6, 17)</t>
+          <t>[3, 6, 17]</t>
         </is>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="n">
         <v>1</v>
@@ -1413,24 +1413,24 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>(4, 8, 9)</t>
+          <t>[4, 8, 9]</t>
         </is>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -1456,17 +1456,17 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>(5, 8, 10)</t>
+          <t>[5, 8, 10]</t>
         </is>
       </c>
       <c r="J24" t="n">
@@ -1499,17 +1499,17 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>(10, 11, 16)</t>
+          <t>[10, 11, 16]</t>
         </is>
       </c>
       <c r="J25" t="n">
@@ -1542,24 +1542,24 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>(6, 7, 23)</t>
+          <t>[6, 7, 23]</t>
         </is>
       </c>
       <c r="J26" t="n">
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>clara</t>
+          <t>pia</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1585,21 +1585,21 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>(6, 7, 23)</t>
+          <t>[6, 7, 23]</t>
         </is>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
         <v>2</v>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>klara</t>
+          <t>sam</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1628,17 +1628,17 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>(9, 11, 19)</t>
+          <t>[9, 11, 19]</t>
         </is>
       </c>
       <c r="J28" t="n">
@@ -1716,59 +1716,59 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>jos</t>
+          <t>luuk</t>
         </is>
       </c>
       <c r="C2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" t="n">
         <v>8</v>
       </c>
-      <c r="D2" t="n">
-        <v>6</v>
-      </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>(6,)</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[2]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(2, 1, 21)</t>
+          <t>[3, 6, 17]</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pol</t>
+          <t>pat</t>
         </is>
       </c>
       <c r="C3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
         <v>7</v>
       </c>
-      <c r="D3" t="n">
-        <v>9</v>
-      </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
@@ -1777,17 +1777,17 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>(1,)</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[1]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>(5, 6, 7)</t>
+          <t>[5, 9, 27]</t>
         </is>
       </c>
       <c r="J3" t="n">
@@ -1817,37 +1817,37 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(6, 7, 23)</t>
+          <t>[6, 7, 23]</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ahmed</t>
+          <t>mo</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -1857,17 +1857,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[3, 8]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>(11,)</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>(12, 5, 25)</t>
+          <t>[12, 5, 25]</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -1876,18 +1876,18 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>pius</t>
+          <t>ahmed</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -1897,34 +1897,34 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>(10,)</t>
+          <t>[11]</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>(2, 4, 6)</t>
+          <t>[12, 5, 25]</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>mario</t>
+          <t>pius</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
         <v>6</v>
@@ -1937,17 +1937,17 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[10]</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>(1, 3, 5)</t>
+          <t>[2, 4, 6]</t>
         </is>
       </c>
       <c r="J7" t="n">
@@ -1956,59 +1956,59 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>pieter</t>
+          <t>mario</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>(2, 1, 21)</t>
+          <t>[1, 3, 5]</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>pieter</t>
+          <t>peter</t>
         </is>
       </c>
       <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="D9" t="n">
         <v>8</v>
       </c>
-      <c r="D9" t="n">
-        <v>7</v>
-      </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
@@ -2017,37 +2017,37 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>(12,)</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>(3, 22, 1)</t>
+          <t>[9, 13, 14]</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>maarten</t>
+          <t>pieter</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -2057,17 +2057,17 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>(3, 6, 17)</t>
+          <t>[3, 22, 1]</t>
         </is>
       </c>
       <c r="J10" t="n">
@@ -2076,78 +2076,78 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>sanne</t>
+          <t>rinus</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>(4, 8, 9)</t>
+          <t>[5, 8, 10]</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>rinus</t>
+          <t>karla</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>(5, 8, 10)</t>
+          <t>[10, 11, 16]</t>
         </is>
       </c>
       <c r="J12" t="n">
@@ -2156,18 +2156,18 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>karla</t>
+          <t>carla</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" t="n">
         <v>-1</v>
@@ -2177,17 +2177,17 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>(10, 11, 16)</t>
+          <t>[6, 7, 23]</t>
         </is>
       </c>
       <c r="J13" t="n">
@@ -2196,18 +2196,18 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>carla</t>
+          <t>pia</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14" t="n">
         <v>-1</v>
@@ -2217,21 +2217,21 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>(6, 7, 23)</t>
+          <t>[6, 7, 23]</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -2242,10 +2242,10 @@
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>7.076923076923077</v>
       </c>
       <c r="D17" t="n">
-        <v>6.769230769230769</v>
+        <v>6.615384615384615</v>
       </c>
       <c r="E17" t="n">
         <v>0.3846153846153846</v>
@@ -2326,59 +2326,59 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>luuk</t>
+          <t>jos</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>(4,)</t>
+          <t>[6]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>(2,)</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(3, 6, 17)</t>
+          <t>[2, 1, 21]</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pat</t>
+          <t>pol</t>
         </is>
       </c>
       <c r="C3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
         <v>9</v>
       </c>
-      <c r="D3" t="n">
-        <v>7</v>
-      </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
@@ -2387,57 +2387,57 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[1]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>(1,)</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>(5, 9, 27)</t>
+          <t>[5, 6, 7]</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>tia</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>6</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>mo</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>5</v>
-      </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(3, 8)</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[8]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(12, 5, 25)</t>
+          <t>[8, 17, 23]</t>
         </is>
       </c>
       <c r="J4" t="n">
@@ -2446,38 +2446,38 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>karl</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>7</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>tia</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>6</v>
-      </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[6]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>(8,)</t>
+          <t>[7]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>(8, 17, 23)</t>
+          <t>[9, 27, 14]</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -2486,18 +2486,18 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>siem</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>8</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>karl</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>7</v>
-      </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -2507,17 +2507,17 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>(6,)</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>(7,)</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>(9, 27, 14)</t>
+          <t>[10, 18, 19]</t>
         </is>
       </c>
       <c r="J6" t="n">
@@ -2526,78 +2526,78 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>siem</t>
+          <t>darius</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[20]</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>(10, 18, 19)</t>
+          <t>[10, 18, 19]</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>darius</t>
+          <t>marius</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>(20,)</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>(10, 18, 19)</t>
+          <t>[5, 6, 7]</t>
         </is>
       </c>
       <c r="J8" t="n">
@@ -2606,58 +2606,58 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>marius</t>
+          <t>maria</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>(5, 6, 7)</t>
+          <t>[5, 6, 7]</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>maria</t>
+          <t>marie</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" t="n">
         <v>-1</v>
@@ -2667,77 +2667,77 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>(5, 6, 7)</t>
+          <t>[3, 6, 17]</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>marie</t>
+          <t>pieter</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>(3, 6, 17)</t>
+          <t>[2, 1, 21]</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>peter</t>
+          <t>pier</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
@@ -2747,17 +2747,17 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>(9, 13, 14)</t>
+          <t>[7, 19, 17]</t>
         </is>
       </c>
       <c r="J12" t="n">
@@ -2766,18 +2766,18 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>pier</t>
+          <t>maarten</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>6</v>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -2787,34 +2787,34 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>(7, 19, 17)</t>
+          <t>[3, 6, 17]</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>clara</t>
+          <t>sanne</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" t="n">
         <v>7</v>
@@ -2827,21 +2827,21 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>(6, 7, 23)</t>
+          <t>[4, 8, 9]</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>klara</t>
+          <t>sam</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -2867,17 +2867,17 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>(9, 11, 19)</t>
+          <t>[9, 11, 19]</t>
         </is>
       </c>
       <c r="J15" t="n">
@@ -2892,10 +2892,10 @@
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>6.928571428571429</v>
       </c>
       <c r="D17" t="n">
-        <v>6.571428571428571</v>
+        <v>6.714285714285714</v>
       </c>
       <c r="E17" t="n">
         <v>0.2857142857142857</v>

</xml_diff>

<commit_message>
moved some files, optimized Dockerfile
</commit_message>
<xml_diff>
--- a/data/web_best_plan.xlsx
+++ b/data/web_best_plan.xlsx
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
         <v>2</v>
@@ -567,10 +567,10 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
         <v>1</v>
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>1</v>
@@ -696,10 +696,10 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -739,7 +739,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
         <v>2</v>
@@ -782,10 +782,10 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -825,10 +825,10 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -871,7 +871,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -914,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -1000,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -1043,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -1083,7 +1083,7 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
         <v>2</v>
@@ -1126,7 +1126,7 @@
         </is>
       </c>
       <c r="J16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="n">
         <v>1</v>
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1212,10 +1212,10 @@
         </is>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -1255,7 +1255,7 @@
         </is>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
         <v>1</v>
@@ -1384,7 +1384,7 @@
         </is>
       </c>
       <c r="J22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" t="n">
         <v>1</v>
@@ -1430,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="K23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1513,10 +1513,10 @@
         </is>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1599,10 +1599,10 @@
         </is>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1642,10 +1642,10 @@
         </is>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1716,59 +1716,59 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>luuk</t>
+          <t>jos</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[6]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[2]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[3, 6, 17]</t>
+          <t>[2, 1, 21]</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pat</t>
+          <t>pol</t>
         </is>
       </c>
       <c r="C3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
         <v>9</v>
       </c>
-      <c r="D3" t="n">
-        <v>7</v>
-      </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
@@ -1777,17 +1777,17 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[1]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[1]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[5, 9, 27]</t>
+          <t>[5, 6, 7]</t>
         </is>
       </c>
       <c r="J3" t="n">
@@ -1796,11 +1796,11 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>katrien</t>
+          <t>tia</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -1822,12 +1822,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[8]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[6, 7, 23]</t>
+          <t>[8, 17, 23]</t>
         </is>
       </c>
       <c r="J4" t="n">
@@ -1836,18 +1836,18 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>mo</t>
+          <t>karl</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -1857,21 +1857,21 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[3, 8]</t>
+          <t>[6]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[7]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[12, 5, 25]</t>
+          <t>[9, 27, 14]</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -1911,7 +1911,7 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -1951,26 +1951,26 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>mario</t>
+          <t>maria</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1987,33 +1987,33 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>[1, 3, 5]</t>
+          <t>[5, 6, 7]</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>peter</t>
+          <t>pieter</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>[9, 13, 14]</t>
+          <t>[2, 1, 21]</t>
         </is>
       </c>
       <c r="J9" t="n">
@@ -2076,19 +2076,19 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>rinus</t>
+          <t>maarten</t>
         </is>
       </c>
       <c r="C11" t="n">
+        <v>6</v>
+      </c>
+      <c r="D11" t="n">
         <v>8</v>
       </c>
-      <c r="D11" t="n">
-        <v>6</v>
-      </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
@@ -2107,30 +2107,30 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>[5, 8, 10]</t>
+          <t>[3, 6, 17]</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>karla</t>
+          <t>rinus</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E12" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>[10, 11, 16]</t>
+          <t>[5, 8, 10]</t>
         </is>
       </c>
       <c r="J12" t="n">
@@ -2196,18 +2196,18 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>pia</t>
+          <t>sam</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" t="n">
         <v>-1</v>
@@ -2227,11 +2227,11 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>[6, 7, 23]</t>
+          <t>[9, 11, 19]</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -2245,7 +2245,7 @@
         <v>7.076923076923077</v>
       </c>
       <c r="D17" t="n">
-        <v>6.615384615384615</v>
+        <v>6.923076923076923</v>
       </c>
       <c r="E17" t="n">
         <v>0.3846153846153846</v>
@@ -2326,59 +2326,59 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>jos</t>
+          <t>luuk</t>
         </is>
       </c>
       <c r="C2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" t="n">
         <v>8</v>
       </c>
-      <c r="D2" t="n">
-        <v>6</v>
-      </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[6]</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[2]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[2, 1, 21]</t>
+          <t>[3, 6, 17]</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pol</t>
+          <t>pat</t>
         </is>
       </c>
       <c r="C3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
         <v>7</v>
       </c>
-      <c r="D3" t="n">
-        <v>9</v>
-      </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
@@ -2387,30 +2387,30 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[5, 6, 7]</t>
+          <t>[5, 9, 27]</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>tia</t>
+          <t>katrien</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -2432,12 +2432,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[8, 17, 23]</t>
+          <t>[6, 7, 23]</t>
         </is>
       </c>
       <c r="J4" t="n">
@@ -2446,18 +2446,18 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>karl</t>
+          <t>mo</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -2467,17 +2467,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[6]</t>
+          <t>[3, 8]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[7]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[9, 27, 14]</t>
+          <t>[12, 5, 25]</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -2521,7 +2521,7 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -2561,7 +2561,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -2601,26 +2601,26 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>maria</t>
+          <t>mario</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -2637,11 +2637,11 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>[5, 6, 7]</t>
+          <t>[1, 3, 5]</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -2681,29 +2681,29 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>pieter</t>
+          <t>peter</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2717,11 +2717,11 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>[2, 1, 21]</t>
+          <t>[9, 13, 14]</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -2766,21 +2766,21 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>maarten</t>
+          <t>sanne</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>[3, 6, 17]</t>
+          <t>[4, 8, 9]</t>
         </is>
       </c>
       <c r="J13" t="n">
@@ -2806,18 +2806,18 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>sanne</t>
+          <t>karla</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E14" t="n">
         <v>-1</v>
@@ -2837,27 +2837,27 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>[4, 8, 9]</t>
+          <t>[10, 11, 16]</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>sam</t>
+          <t>pia</t>
         </is>
       </c>
       <c r="C15" t="n">
+        <v>6</v>
+      </c>
+      <c r="D15" t="n">
         <v>7</v>
-      </c>
-      <c r="D15" t="n">
-        <v>8</v>
       </c>
       <c r="E15" t="n">
         <v>-1</v>
@@ -2877,11 +2877,11 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>[9, 11, 19]</t>
+          <t>[6, 7, 23]</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -2895,7 +2895,7 @@
         <v>6.928571428571429</v>
       </c>
       <c r="D17" t="n">
-        <v>6.714285714285714</v>
+        <v>6.428571428571429</v>
       </c>
       <c r="E17" t="n">
         <v>0.2857142857142857</v>

</xml_diff>